<commit_message>
add generate noise trajectory
</commit_message>
<xml_diff>
--- a/basin_diff_barrier_to_noise.xlsx
+++ b/basin_diff_barrier_to_noise.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6294642857142857</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4375</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7589285714285714</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5625</v>
+        <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7008928571428571</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.96875</v>
+        <v>0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.84375</v>
+        <v>0.5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8839285714285714</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.859375</v>
+        <v>0.75</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8861607142857143</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.96875</v>
+        <v>0.5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3125</v>
+        <v>0.5</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7767857142857143</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.90625</v>
+        <v>0.25</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9196428571428571</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.96875</v>
+        <v>0.25</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6696428571428571</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.125</v>
+        <v>0.75</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.484375</v>
+        <v>0.5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7388392857142857</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.96875</v>
+        <v>0.25</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5625</v>
+        <v>0.5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7767857142857143</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.71875</v>
+        <v>0.75</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7991071428571429</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9375</v>
+        <v>0.5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9508928571428571</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.828125</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8370535714285714</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.890625</v>
+        <v>0.5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9174107142857143</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.953125</v>
+        <v>0.25</v>
       </c>
       <c r="C23" t="n">
-        <v>0.953125</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.78125</v>
+        <v>0.5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8660714285714286</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.78125</v>
+        <v>0.5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8705357142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9375</v>
+        <v>0.5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9553571428571429</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.90625</v>
+        <v>0.75</v>
       </c>
       <c r="C27" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.71875</v>
+        <v>0.5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7901785714285714</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6116071428571429</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.59375</v>
+        <v>0.5</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7589285714285714</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.046875</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.5424107142857143</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="32">
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C32" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="33">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.984375</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.984375</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="34">
@@ -802,10 +802,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.84375</v>
+        <v>0.25</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="35">
@@ -813,10 +813,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.734375</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0.8102678571428571</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="36">
@@ -824,10 +824,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.15625</v>
+        <v>0.5</v>
       </c>
       <c r="C36" t="n">
-        <v>0.65625</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="37">
@@ -835,10 +835,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.78125</v>
+        <v>0.5</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8214285714285714</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38">
@@ -846,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="39">
@@ -857,10 +857,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
         <v>0.25</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.6785714285714286</v>
       </c>
     </row>
     <row r="40">
@@ -868,10 +868,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.984375</v>
+        <v>0.5</v>
       </c>
       <c r="C40" t="n">
-        <v>0.984375</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="41">
@@ -879,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.265625</v>
+        <v>0.75</v>
       </c>
       <c r="C41" t="n">
-        <v>0.5647321428571429</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="42">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.578125</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>0.734375</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="43">
@@ -901,10 +901,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6517857142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44">
@@ -912,10 +912,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.84375</v>
+        <v>0.25</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9017857142857143</v>
+        <v>0.2222222222222222</v>
       </c>
     </row>
     <row r="45">
@@ -923,10 +923,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.078125</v>
+        <v>0.75</v>
       </c>
       <c r="C45" t="n">
-        <v>0.5736607142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46">
@@ -934,10 +934,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.6875</v>
+        <v>0.5</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7723214285714286</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="47">
@@ -945,10 +945,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.84375</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="48">
@@ -956,10 +956,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.921875</v>
+        <v>0.5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.9397321428571429</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49">
@@ -967,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C49" t="n">
-        <v>0.6696428571428571</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="50">
@@ -978,10 +978,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.96875</v>
+        <v>0.25</v>
       </c>
       <c r="C50" t="n">
-        <v>0.96875</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="51">
@@ -989,10 +989,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.046875</v>
+        <v>0.5</v>
       </c>
       <c r="C51" t="n">
-        <v>0.6004464285714286</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="52">
@@ -1003,7 +1003,7 @@
         <v>0.75</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="53">
@@ -1011,10 +1011,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3125</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.6383928571428571</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54">
@@ -1022,10 +1022,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.671875</v>
+        <v>0.75</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7120535714285714</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="55">
@@ -1033,10 +1033,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.21875</v>
+        <v>0.5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.5580357142857143</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="56">
@@ -1044,10 +1044,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.984375</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.984375</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="57">
@@ -1055,10 +1055,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58">
@@ -1066,10 +1066,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="59">
@@ -1077,10 +1077,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.21875</v>
+        <v>0.25</v>
       </c>
       <c r="C59" t="n">
-        <v>0.6607142857142857</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="60">
@@ -1088,10 +1088,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="61">
@@ -1099,10 +1099,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.84375</v>
+        <v>0.75</v>
       </c>
       <c r="C61" t="n">
-        <v>0.8660714285714286</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="62">
@@ -1110,10 +1110,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.7276785714285714</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="63">
@@ -1121,10 +1121,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.34375</v>
+        <v>0.5</v>
       </c>
       <c r="C63" t="n">
-        <v>0.6517857142857143</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64">
@@ -1132,10 +1132,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.6651785714285714</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="65">
@@ -1143,10 +1143,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.921875</v>
+        <v>0.75</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9397321428571429</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="66">
@@ -1154,10 +1154,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.53125</v>
+        <v>0.75</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7321428571428571</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="67">
@@ -1165,10 +1165,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.78125</v>
+        <v>0.75</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8482142857142857</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="68">
@@ -1176,10 +1176,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.984375</v>
+        <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.984375</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="69">
@@ -1187,10 +1187,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.6875</v>
+        <v>0.5</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7946428571428571</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="70">
@@ -1198,10 +1198,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.125</v>
+        <v>0.75</v>
       </c>
       <c r="C70" t="n">
-        <v>0.7589285714285714</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="71">
@@ -1209,10 +1209,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.1875</v>
+        <v>0.75</v>
       </c>
       <c r="C71" t="n">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="72">
@@ -1220,10 +1220,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.4375</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7410714285714286</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="73">
@@ -1231,10 +1231,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.15625</v>
+        <v>0.5</v>
       </c>
       <c r="C73" t="n">
-        <v>0.6964285714285714</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74">
@@ -1242,10 +1242,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.6875</v>
+        <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.8035714285714286</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="75">
@@ -1253,10 +1253,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.40625</v>
+        <v>0.5</v>
       </c>
       <c r="C75" t="n">
-        <v>0.5848214285714286</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="76">
@@ -1264,10 +1264,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.890625</v>
+        <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9084821428571429</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="77">
@@ -1275,10 +1275,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.734375</v>
+        <v>0.5</v>
       </c>
       <c r="C77" t="n">
-        <v>0.8459821428571429</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="78">
@@ -1286,10 +1286,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.96875</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="79">
@@ -1297,10 +1297,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.046875</v>
+        <v>0.5</v>
       </c>
       <c r="C79" t="n">
-        <v>0.4084821428571428</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="80">
@@ -1308,10 +1308,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.84375</v>
+        <v>0.5</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="81">
@@ -1319,10 +1319,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.921875</v>
+        <v>0.75</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9352678571428571</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="82">
@@ -1330,10 +1330,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.96875</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9732142857142857</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="83">
@@ -1341,10 +1341,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.15625</v>
+        <v>0.75</v>
       </c>
       <c r="C83" t="n">
-        <v>0.6517857142857143</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="84">
@@ -1352,10 +1352,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.78125</v>
+        <v>0.5</v>
       </c>
       <c r="C84" t="n">
-        <v>0.8125</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="85">
@@ -1363,10 +1363,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="86">
@@ -1374,10 +1374,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.5625</v>
+        <v>0.75</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7098214285714286</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="87">
@@ -1385,10 +1385,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.78125</v>
+        <v>0.5</v>
       </c>
       <c r="C87" t="n">
-        <v>0.8348214285714286</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="88">
@@ -1396,10 +1396,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.09375</v>
+        <v>0.75</v>
       </c>
       <c r="C88" t="n">
-        <v>0.6517857142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="89">
@@ -1407,10 +1407,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.8125</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.875</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="90">
@@ -1418,10 +1418,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0625</v>
+        <v>0.5</v>
       </c>
       <c r="C90" t="n">
-        <v>0.7053571428571429</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="91">
@@ -1429,10 +1429,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.9375</v>
+        <v>0.75</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9553571428571429</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="92">
@@ -1440,10 +1440,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.9375</v>
+        <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9553571428571429</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="93">
@@ -1451,10 +1451,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="C93" t="n">
-        <v>0.5982142857142857</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="94">
@@ -1462,10 +1462,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.15625</v>
+        <v>0.25</v>
       </c>
       <c r="C94" t="n">
-        <v>0.5491071428571429</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="95">
@@ -1473,10 +1473,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.921875</v>
+        <v>0.5</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9397321428571429</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="96">
@@ -1484,10 +1484,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.6607142857142857</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="97">
@@ -1495,10 +1495,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.890625</v>
+        <v>0.5</v>
       </c>
       <c r="C97" t="n">
-        <v>0.9084821428571429</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="98">
@@ -1509,7 +1509,7 @@
         <v>0.75</v>
       </c>
       <c r="C98" t="n">
-        <v>0.8080357142857143</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="99">
@@ -1517,10 +1517,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.34375</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.59375</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="100">
@@ -1528,10 +1528,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.890625</v>
+        <v>0.5</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9084821428571429</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
     <row r="101">
@@ -1539,10 +1539,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.9375</v>
+        <v>0.5</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9464285714285714</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>